<commit_message>
class build2 update done
</commit_message>
<xml_diff>
--- a/dev/doc/class.xlsx
+++ b/dev/doc/class.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'build1-2'!$A$1:$J$69</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'build2-3'!$A$1:$J$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'build2-3'!$A$1:$J$76</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="507">
   <si>
     <t>logic</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -4220,12 +4220,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>新建类：
-1. layout设置
-2. 实现选择player和campaign的功能</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>陈思羽、齐锴</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4320,10 +4314,6 @@
   </si>
   <si>
     <t>1. build2 里面有关 map loading的测试，是不是应该单独拿一个方法出来？</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>新增</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -4845,6 +4835,34 @@
 3.注意delegate和observer关系处理
 4.穿卸装备对attribute的影响实现
 5.level在0-20之间才能set</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建类：
+1. layout设置
+2. 实现选择player和campaign的功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishScene</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建类：
+campaign结束后的界面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈思羽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增：
+TestSuite类</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>目前其他的delegate内的抽象方法名字都是**PerformAction格式，建议将方法gameMapViewSelect()改名为gameMapViewSelectPerformAction()，否则在实现类里，不能一眼看出这个是一个delegate的实现方法</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -7016,13 +7034,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
+      <selection pane="bottomRight" activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -7072,10 +7090,10 @@
         <v>415</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>456</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>457</v>
       </c>
       <c r="M1" s="37" t="s">
         <v>416</v>
@@ -7181,10 +7199,10 @@
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="29" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1">
@@ -7207,7 +7225,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="29" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J7" s="38" t="s">
         <v>199</v>
@@ -7266,13 +7284,13 @@
         <v>95</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="J10" s="38" t="s">
         <v>200</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="34.5" customHeight="1">
@@ -7295,7 +7313,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="34.5" customHeight="1">
@@ -7348,7 +7366,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="29" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>432</v>
@@ -7367,7 +7385,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="29" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>432</v>
@@ -7389,7 +7407,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="29" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>432</v>
@@ -7411,7 +7429,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="29" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>432</v>
@@ -7433,7 +7451,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>432</v>
@@ -7710,7 +7728,7 @@
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="29" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J32" s="39" t="s">
         <v>201</v>
@@ -7734,7 +7752,7 @@
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J33" s="39" t="s">
         <v>202</v>
@@ -7758,7 +7776,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J34" s="39" t="s">
         <v>202</v>
@@ -7906,7 +7924,7 @@
         <v>171</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J40" s="39" t="s">
         <v>201</v>
@@ -7930,7 +7948,7 @@
       <c r="G41" s="18"/>
       <c r="H41" s="10"/>
       <c r="I41" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J41" s="39" t="s">
         <v>201</v>
@@ -7964,7 +7982,7 @@
         <v>200</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="34.5" customHeight="1">
@@ -8008,7 +8026,7 @@
         <v>178</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="J44" s="39" t="s">
         <v>219</v>
@@ -8121,7 +8139,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="30" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="J49" s="39" t="s">
         <v>201</v>
@@ -8173,7 +8191,7 @@
         <v>211</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J51" s="39" t="s">
         <v>437</v>
@@ -8259,10 +8277,10 @@
       <c r="G55" s="18"/>
       <c r="H55" s="10"/>
       <c r="I55" s="29" t="s">
+        <v>501</v>
+      </c>
+      <c r="J55" s="39" t="s">
         <v>447</v>
-      </c>
-      <c r="J55" s="39" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="34.5" customHeight="1">
@@ -8283,90 +8301,93 @@
       <c r="G56" s="18"/>
       <c r="H56" s="10"/>
       <c r="I56" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="J56" s="43" t="s">
         <v>449</v>
-      </c>
-      <c r="J56" s="43" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="34.5" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>502</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E57" s="10"/>
-      <c r="F57" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>176</v>
-      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="18"/>
       <c r="H57" s="10"/>
-      <c r="J57" s="2"/>
+      <c r="I57" s="29" t="s">
+        <v>503</v>
+      </c>
+      <c r="J57" s="43" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="58" spans="1:10" ht="34.5" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>180</v>
-      </c>
+      <c r="F58" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" s="10"/>
       <c r="J58" s="2"/>
     </row>
     <row r="59" spans="1:10" ht="34.5" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>28</v>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="E59" s="10"/>
-      <c r="F59" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="H59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="J59" s="2"/>
     </row>
     <row r="60" spans="1:10" ht="34.5" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>67</v>
+      <c r="B60" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="18" t="s">
-        <v>174</v>
+      <c r="F60" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="H60" s="10"/>
       <c r="J60" s="2"/>
@@ -8376,18 +8397,16 @@
         <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E61" s="10"/>
-      <c r="F61" s="10" t="s">
-        <v>172</v>
-      </c>
+      <c r="F61" s="10"/>
       <c r="G61" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H61" s="10"/>
       <c r="J61" s="2"/>
@@ -8397,13 +8416,18 @@
         <v>66</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C62" s="8"/>
+      <c r="D62" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="G62" s="18" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H62" s="10"/>
       <c r="J62" s="2"/>
@@ -8413,16 +8437,13 @@
         <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C63" s="8"/>
-      <c r="D63" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
       <c r="G63" s="18" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H63" s="10"/>
       <c r="J63" s="2"/>
@@ -8432,7 +8453,7 @@
         <v>66</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8" t="s">
@@ -8440,18 +8461,18 @@
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
-      <c r="G64" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="H64" s="18"/>
+      <c r="G64" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="H64" s="10"/>
       <c r="J64" s="2"/>
     </row>
     <row r="65" spans="1:11" ht="34.5" customHeight="1">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="36" t="s">
-        <v>21</v>
+      <c r="B65" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8" t="s">
@@ -8459,23 +8480,18 @@
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
-      <c r="G65" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="H65" s="10"/>
-      <c r="I65" s="29" t="s">
-        <v>452</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>205</v>
-      </c>
+      <c r="G65" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="H65" s="18"/>
+      <c r="J65" s="2"/>
     </row>
     <row r="66" spans="1:11" ht="34.5" customHeight="1">
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8" t="s">
@@ -8484,41 +8500,59 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
       <c r="G66" s="18" t="s">
-        <v>445</v>
-      </c>
-      <c r="H66" s="18" t="s">
-        <v>210</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="H66" s="10"/>
       <c r="I66" s="29" t="s">
-        <v>204</v>
+        <v>451</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="H67" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="I67" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K67" s="29" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="34.5" customHeight="1">
+      <c r="A68" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F68" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G67" s="10" t="s">
+      <c r="G68" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="H67" s="10"/>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="H68" s="10"/>
       <c r="J68" s="2"/>
     </row>
     <row r="69" spans="1:11" ht="34.5" customHeight="1">
@@ -8526,23 +8560,20 @@
         <v>159</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J69" s="2"/>
-      <c r="K69" s="44" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="70" spans="1:11" ht="34.5" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="44" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="34.5" customHeight="1">
@@ -8550,75 +8581,84 @@
         <v>159</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J71" s="2"/>
-      <c r="K71" s="45" t="s">
-        <v>455</v>
+      <c r="K71" s="44" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="34.5" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B72" s="40" t="s">
-        <v>453</v>
-      </c>
-      <c r="I72" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="K72" s="44" t="s">
-        <v>474</v>
+      <c r="B72" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J72" s="2"/>
+      <c r="K72" s="45" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="34.5" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B73" s="40" t="s">
+        <v>452</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="J73" s="2"/>
-      <c r="K73" s="29" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="29.25">
+      <c r="K73" s="44" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="34.5" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B74" s="40" t="s">
+      <c r="B74" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="J74" s="2"/>
+      <c r="K74" s="29" t="s">
         <v>458</v>
-      </c>
-      <c r="I74" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="29.25">
       <c r="A75" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>457</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="29.25">
+      <c r="A76" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B76" s="40" t="s">
         <v>460</v>
       </c>
-      <c r="B75" s="40" t="s">
-        <v>461</v>
-      </c>
-      <c r="I75" s="29" t="s">
-        <v>466</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="K75" s="29" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="J76" s="39"/>
+      <c r="I76" s="29" t="s">
+        <v>505</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="K76" s="29" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="77" spans="1:11">
       <c r="J77" s="39"/>
@@ -8626,8 +8666,11 @@
     <row r="78" spans="1:11">
       <c r="J78" s="39"/>
     </row>
+    <row r="79" spans="1:11">
+      <c r="J79" s="39"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J75"/>
+  <autoFilter ref="A1:J76"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8652,64 +8695,64 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="46" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="57">
       <c r="A2" s="49" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="71.25">
       <c r="A3" s="49" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="42.75">
       <c r="A4" s="49" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="11" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="99.75">
       <c r="A5" s="49" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="71.25">
       <c r="A6" s="49" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>